<commit_message>
Remove warnings and fix IYCF
</commit_message>
<xml_diff>
--- a/analyses/inputs/Medium 2019 base/Afghanistan_input.xlsx
+++ b/analyses/inputs/Medium 2019 base/Afghanistan_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\Nutrition\analyses\inputs\Medium 2019 base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{582E1DF8-AD73-4C0E-9EF3-F8FAC742A9AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{406BA644-19F3-45F3-89BB-A12EF121B857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17196" yWindow="-13068" windowWidth="23256" windowHeight="12576" tabRatio="961" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17196" yWindow="-13068" windowWidth="23256" windowHeight="12576" tabRatio="961" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="272">
   <si>
     <t>year</t>
   </si>
@@ -12893,12 +12893,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -12908,6 +12902,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -21408,7 +21408,7 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -21637,8 +21637,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
@@ -21685,10 +21685,10 @@
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="81"/>
+      <c r="D3" s="81" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="81"/>
       <c r="E3" s="58" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -21699,10 +21699,10 @@
       <c r="B4" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="81" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="81"/>
       <c r="E4" s="58" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -21713,9 +21713,7 @@
       <c r="B5" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="81" t="s">
-        <v>216</v>
-      </c>
+      <c r="C5" s="81"/>
       <c r="D5" s="81"/>
       <c r="E5" s="58" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -21727,9 +21725,7 @@
       <c r="B6" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="81" t="s">
-        <v>216</v>
-      </c>
+      <c r="C6" s="81"/>
       <c r="D6" s="81"/>
       <c r="E6" s="58" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -21762,9 +21758,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="81"/>
-      <c r="D10" s="81" t="s">
-        <v>216</v>
-      </c>
+      <c r="D10" s="81"/>
       <c r="E10" s="58"/>
     </row>
     <row r="11" spans="1:5">
@@ -21773,9 +21767,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="81"/>
-      <c r="D11" s="81" t="s">
-        <v>216</v>
-      </c>
+      <c r="D11" s="81"/>
       <c r="E11" s="58"/>
     </row>
     <row r="12" spans="1:5">

</xml_diff>

<commit_message>
Fix IPTp and MMS costs
</commit_message>
<xml_diff>
--- a/analyses/inputs/Medium 2019 base/Afghanistan_input.xlsx
+++ b/analyses/inputs/Medium 2019 base/Afghanistan_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\Nutrition\analyses\inputs\Medium 2019 base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7A39B28-6AA5-4C1E-BAC9-FBC249187D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F080143-1EC8-4A55-9135-BADD35077B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="-18270" windowWidth="29040" windowHeight="17640" tabRatio="961" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22148,7 +22148,7 @@
         <v>0.95</v>
       </c>
       <c r="D11" s="86">
-        <v>1.47</v>
+        <v>1.39</v>
       </c>
       <c r="E11" s="86" t="s">
         <v>201</v>
@@ -22165,7 +22165,7 @@
         <v>0.95</v>
       </c>
       <c r="D12" s="86">
-        <v>1.47</v>
+        <v>1.39</v>
       </c>
       <c r="E12" s="86" t="s">
         <v>201</v>
@@ -22182,7 +22182,7 @@
         <v>0.95</v>
       </c>
       <c r="D13" s="86">
-        <v>1.47</v>
+        <v>1.39</v>
       </c>
       <c r="E13" s="86" t="s">
         <v>201</v>
@@ -22216,7 +22216,7 @@
         <v>0.95</v>
       </c>
       <c r="D15" s="86">
-        <v>19.47</v>
+        <v>18.37</v>
       </c>
       <c r="E15" s="86" t="s">
         <v>201</v>
@@ -22233,7 +22233,7 @@
         <v>0.95</v>
       </c>
       <c r="D16" s="86">
-        <v>0.15</v>
+        <v>0.27</v>
       </c>
       <c r="E16" s="86" t="s">
         <v>201</v>
@@ -22250,7 +22250,7 @@
         <v>0.95</v>
       </c>
       <c r="D17" s="86">
-        <v>0.27</v>
+        <v>0.15</v>
       </c>
       <c r="E17" s="86" t="s">
         <v>201</v>
@@ -22284,7 +22284,7 @@
         <v>0.95</v>
       </c>
       <c r="D19" s="86">
-        <v>1.58</v>
+        <v>1.49</v>
       </c>
       <c r="E19" s="86" t="s">
         <v>201</v>
@@ -22420,7 +22420,7 @@
         <v>0.95</v>
       </c>
       <c r="D27" s="86">
-        <v>4.07</v>
+        <v>26.56</v>
       </c>
       <c r="E27" s="86" t="s">
         <v>201</v>
@@ -22488,7 +22488,7 @@
         <v>0.95</v>
       </c>
       <c r="D31" s="86">
-        <v>236.93</v>
+        <v>223.52</v>
       </c>
       <c r="E31" s="86" t="s">
         <v>201</v>

</xml_diff>

<commit_message>
PPCF interaction with IYCF
</commit_message>
<xml_diff>
--- a/analyses/inputs/Medium 2019 base/Afghanistan_input.xlsx
+++ b/analyses/inputs/Medium 2019 base/Afghanistan_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\Nutrition\analyses\inputs\Medium 2019 base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F080143-1EC8-4A55-9135-BADD35077B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1942B4E-4449-4336-98C5-9D2DBEFC2B94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="-18270" windowWidth="29040" windowHeight="17640" tabRatio="961" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="-18270" windowWidth="29040" windowHeight="17640" tabRatio="961" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="272">
   <si>
     <t>year</t>
   </si>
@@ -6202,7 +6202,7 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -6679,7 +6679,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6738,8 +6738,12 @@
       <c r="C5" s="81"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="87"/>
+      <c r="A6" s="89" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="87" t="s">
+        <v>58</v>
+      </c>
       <c r="C6" s="87"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -11782,8 +11786,8 @@
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12461,7 +12465,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="105">
-        <v>0.78</v>
+        <v>0.89</v>
       </c>
       <c r="H31" s="105">
         <v>1</v>
@@ -12482,7 +12486,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="105">
-        <v>0.78</v>
+        <v>0.89</v>
       </c>
       <c r="H32" s="105">
         <v>1</v>
@@ -12893,12 +12897,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -12908,6 +12906,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -21408,7 +21412,7 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -21952,8 +21956,8 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView zoomScale="106" workbookViewId="0">
-      <selection activeCell="D39" sqref="D2:D39"/>
+    <sheetView topLeftCell="A13" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22281,7 +22285,8 @@
         <v>0.24299999999999999</v>
       </c>
       <c r="C19" s="85">
-        <v>0.95</v>
+        <f>(1-food_insecure)*0.95</f>
+        <v>0.50131500000000007</v>
       </c>
       <c r="D19" s="86">
         <v>1.49</v>

</xml_diff>

<commit_message>
SAM treatment as a reference program
</commit_message>
<xml_diff>
--- a/analyses/inputs/Medium 2019 base/Afghanistan_input.xlsx
+++ b/analyses/inputs/Medium 2019 base/Afghanistan_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\Nutrition\analyses\inputs\Medium 2019 base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1942B4E-4449-4336-98C5-9D2DBEFC2B94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F2C77AD-CD14-426D-A694-1C5311F1AC53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="-18270" windowWidth="29040" windowHeight="17640" tabRatio="961" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12465" yWindow="-13875" windowWidth="23250" windowHeight="12570" tabRatio="961" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="272">
   <si>
     <t>year</t>
   </si>
@@ -6857,8 +6857,8 @@
   </sheetPr>
   <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6913,7 +6913,9 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
+      <c r="A10" s="48" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="48"/>
@@ -11786,7 +11788,7 @@
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -12897,6 +12899,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -12906,12 +12914,6 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
CCT constrained by PPCF
</commit_message>
<xml_diff>
--- a/analyses/inputs/Medium 2019 base/Afghanistan_input.xlsx
+++ b/analyses/inputs/Medium 2019 base/Afghanistan_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\Nutrition\analyses\inputs\Medium 2019 base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D276027A-B244-48E1-ADF5-DE4B56B21668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B7B4DE4-5107-448F-B7A3-7E06507B14D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="-18270" windowWidth="29040" windowHeight="17640" tabRatio="961" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22052,7 +22052,7 @@
         <v>0.95</v>
       </c>
       <c r="D4" s="86">
-        <v>3.39</v>
+        <v>1.91</v>
       </c>
       <c r="E4" s="86" t="s">
         <v>201</v>
@@ -22325,7 +22325,7 @@
         <v>0.95</v>
       </c>
       <c r="D20" s="86">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E20" s="86" t="s">
         <v>201</v>

</xml_diff>